<commit_message>
20200615_- excel, msgbox, icon ,beautify, ip_setting
</commit_message>
<xml_diff>
--- a/GUI_services.xlsx
+++ b/GUI_services.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\柯奇\py\Office_Guidace_System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Koach\Desktop\Office_guidace_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF766977-4AB1-49C0-90B4-AF46A4E4CA1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="13920" yWindow="1425" windowWidth="11385" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>項目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -71,13 +72,21 @@
   </si>
   <si>
     <t>休學、復學、退學申請</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分機號碼</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -395,68 +404,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>123123</v>
+      </c>
+      <c r="C2">
+        <v>22222</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>123123</v>
+      </c>
+      <c r="C3">
+        <v>22222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>22222</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>123123</v>
+      </c>
+      <c r="C5">
+        <v>22222</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>123123</v>
+      </c>
+      <c r="C6">
+        <v>22222</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>22222</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>123123</v>
+      </c>
+      <c r="C8">
+        <v>22222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+      <c r="C9">
+        <v>22222</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
20200617 update binding hyperlink
</commit_message>
<xml_diff>
--- a/GUI_services.xlsx
+++ b/GUI_services.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Koach\Desktop\Office_guidace_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF766977-4AB1-49C0-90B4-AF46A4E4CA1A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4546B46F-B4D5-4CB5-8762-2991B8C91987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13920" yWindow="1425" windowWidth="11385" windowHeight="13245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="工作表2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>項目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -59,27 +60,66 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>請準備護照影本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>請準備身分證影本</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>其他(請填寫內容)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>休學、復學、退學申請</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>test</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>分機號碼</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請填寫各項證明文件申請表，並至綜合行政組繳費，繳完費將繳費單及收據交給承辦人為您處理，謝謝</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請親自至校務系統 - 查詢 - 在學證明書列印 - 點選列印再由承辦人員為您蓋章</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>請同學拿出學生證以方便確認學生身分</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>櫃台</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>科系</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分機</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>問題諮詢</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>其他</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>學生變更基本資料</t>
+  </si>
+  <si>
+    <t>選課相關</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>抵免、抵充申請</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工讀生</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>承辦人</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>v</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -405,121 +445,209 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="2" max="2" width="107.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2">
+        <v>22222</v>
+      </c>
+      <c r="D2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>22222</v>
+      </c>
+      <c r="D3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>22222</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>22222</v>
+      </c>
+      <c r="D5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>22222</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>22222</v>
+      </c>
+      <c r="D7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8">
+        <v>123123</v>
+      </c>
+      <c r="C8">
+        <v>22222</v>
+      </c>
+      <c r="D8" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>123</v>
+      </c>
+      <c r="C9">
+        <v>22222</v>
+      </c>
+      <c r="D9" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FFE43A-95EE-493F-B84A-69FE88329AAF}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2">
-        <v>123123</v>
-      </c>
-      <c r="C2">
-        <v>22222</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3">
-        <v>123123</v>
-      </c>
-      <c r="C3">
-        <v>22222</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4">
-        <v>22222</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
-        <v>123123</v>
-      </c>
-      <c r="C5">
-        <v>22222</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6">
-        <v>123123</v>
-      </c>
-      <c r="C6">
-        <v>22222</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7">
-        <v>22222</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8">
-        <v>123123</v>
-      </c>
-      <c r="C8">
-        <v>22222</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9">
-        <v>123</v>
-      </c>
-      <c r="C9">
-        <v>22222</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
20200617 data link done need to set request frame
</commit_message>
<xml_diff>
--- a/GUI_services.xlsx
+++ b/GUI_services.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Koach\Desktop\Office_guidace_System\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\柯奇\py\office_guidance_sys\Office_Guidance_System\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4546B46F-B4D5-4CB5-8762-2991B8C91987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>項目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -64,10 +63,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>分機號碼</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>請填寫各項證明文件申請表，並至綜合行政組繳費，繳完費將繳費單及收據交給承辦人為您處理，謝謝</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -108,25 +103,13 @@
   </si>
   <si>
     <t>抵免、抵充申請</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>工讀生</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>承辦人</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>v</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -444,11 +427,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C1" sqref="C1:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -458,168 +441,96 @@
     <col min="3" max="3" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2">
-        <v>22222</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3">
-        <v>22222</v>
-      </c>
-      <c r="D3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>22222</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>22222</v>
-      </c>
-      <c r="D5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>22222</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>22222</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>123123</v>
       </c>
-      <c r="C8">
-        <v>22222</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B9">
         <v>123</v>
       </c>
-      <c r="C9">
-        <v>22222</v>
-      </c>
-      <c r="D9" t="s">
-        <v>23</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
-      </c>
-      <c r="D10" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -630,7 +541,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91FFE43A-95EE-493F-B84A-69FE88329AAF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -641,13 +552,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0619 network exception setting
</commit_message>
<xml_diff>
--- a/GUI_services.xlsx
+++ b/GUI_services.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>項目</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -206,8 +206,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
@@ -491,7 +492,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:B27"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -602,15 +603,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -620,224 +621,287 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="1">
         <v>2</v>
       </c>
       <c r="C2">
+        <v>22222</v>
+      </c>
+      <c r="D2">
         <v>12812</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>21</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>2</v>
       </c>
       <c r="C3">
+        <v>22222</v>
+      </c>
+      <c r="D3">
         <v>12812</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>2</v>
       </c>
       <c r="C4">
+        <v>22222</v>
+      </c>
+      <c r="D4">
         <v>12812</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>8</v>
       </c>
       <c r="C5">
+        <v>22222</v>
+      </c>
+      <c r="D5">
         <v>12813</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>24</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>8</v>
       </c>
       <c r="C6">
+        <v>22222</v>
+      </c>
+      <c r="D6">
         <v>12813</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>25</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="1">
         <v>8</v>
       </c>
       <c r="C7">
+        <v>22222</v>
+      </c>
+      <c r="D7">
         <v>12813</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="1">
         <v>7</v>
       </c>
       <c r="C8">
+        <v>22222</v>
+      </c>
+      <c r="D8">
         <v>12814</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>27</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="1">
         <v>7</v>
       </c>
       <c r="C9">
+        <v>22222</v>
+      </c>
+      <c r="D9">
         <v>12814</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>28</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="1">
         <v>7</v>
       </c>
       <c r="C10">
+        <v>22222</v>
+      </c>
+      <c r="D10">
         <v>12814</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="1">
         <v>6</v>
       </c>
       <c r="C11">
+        <v>22222</v>
+      </c>
+      <c r="D11">
         <v>12816</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>30</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>6</v>
       </c>
       <c r="C12">
+        <v>22222</v>
+      </c>
+      <c r="D12">
         <v>12816</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>31</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="1">
         <v>6</v>
       </c>
       <c r="C13">
+        <v>22222</v>
+      </c>
+      <c r="D13">
         <v>12816</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>32</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14">
+        <v>22222</v>
+      </c>
+      <c r="D14">
         <v>12817</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>33</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="1">
         <v>1</v>
       </c>
       <c r="C15">
+        <v>22222</v>
+      </c>
+      <c r="D15">
         <v>12817</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="1">
         <v>1</v>
       </c>
       <c r="C16">
+        <v>22222</v>
+      </c>
+      <c r="D16">
         <v>12817</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="1">
         <v>6.5</v>
       </c>
       <c r="C17">
+        <v>22222</v>
+      </c>
+      <c r="D17">
         <v>12818</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="1">
         <v>6.5</v>
       </c>
       <c r="C18">
+        <v>22222</v>
+      </c>
+      <c r="D18">
         <v>12818</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>5</v>
       </c>
       <c r="C19">
+        <v>22222</v>
+      </c>
+      <c r="D19">
         <v>12815</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="1">
         <v>0</v>
       </c>
       <c r="C20">
+        <v>22222</v>
+      </c>
+      <c r="D20">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="1">
         <v>0</v>
       </c>
       <c r="C21">
+        <v>22222</v>
+      </c>
+      <c r="D21">
         <v>0</v>
       </c>
     </row>

</xml_diff>